<commit_message>
Updated hardcoded script and new output
</commit_message>
<xml_diff>
--- a/CDE_ID_detective_revamp/KnowledgeBase/Compiled_CORE_CDEs list_English_one sheet_as of 2025-01-28.xlsx
+++ b/CDE_ID_detective_revamp/KnowledgeBase/Compiled_CORE_CDEs list_English_one sheet_as of 2025-01-28.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmaefos\Code Stuffs\CDE_detective\CDE_ID_detective_revamp\KnowledgeBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC88380-F75B-42B8-A419-4A6A3AB1FA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557A7513-1F25-4B5D-A687-6554F651F309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38505" yWindow="6465" windowWidth="20265" windowHeight="20985" activeTab="1" xr2:uid="{35A4921A-9D1F-4A50-94BD-2A3998B45EE8}"/>
+    <workbookView xWindow="-38505" yWindow="6465" windowWidth="20265" windowHeight="20985" xr2:uid="{35A4921A-9D1F-4A50-94BD-2A3998B45EE8}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -16661,7 +16661,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{06BF0BB1-AF18-42F5-A5F1-83AA7DF4D85D}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{06BF0BB1-AF18-42F5-A5F1-83AA7DF4D85D}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:A80" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="24">
     <pivotField showAll="0"/>
@@ -17944,9 +17944,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F8D453-0289-4E16-AB7B-CD7D302713CA}">
   <dimension ref="A1:Y435"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A392" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E412" sqref="E412"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A371" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E381" sqref="E381"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -41117,7 +41117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B03DD75-91C1-4925-A600-9AD1195ECA81}">
   <dimension ref="A3:A80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
@@ -41522,6 +41522,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3ebfc1ff-6854-40f8-8577-9c1c65c79578" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D5B4F2C3D199264E8B8F6DBDBC9FDDAA" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e6ed8d6e314981ace17ace03515ae845">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3ebfc1ff-6854-40f8-8577-9c1c65c79578" xmlns:ns4="1db1eb16-7f87-45b5-a5c6-bd3f038db8d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a14e8e53890f120b2bee09526d13603f" ns3:_="" ns4:_="">
     <xsd:import namespace="3ebfc1ff-6854-40f8-8577-9c1c65c79578"/>
@@ -41710,24 +41727,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3DFAF0B-A9BC-422F-A722-23A769C31190}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="1db1eb16-7f87-45b5-a5c6-bd3f038db8d0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="3ebfc1ff-6854-40f8-8577-9c1c65c79578"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3ebfc1ff-6854-40f8-8577-9c1c65c79578" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DFF46F5-41AA-471B-8C04-D49580FCB34E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DDD3AD7-7B2B-4497-B765-450837BD813B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -41744,29 +41769,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DFF46F5-41AA-471B-8C04-D49580FCB34E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3DFAF0B-A9BC-422F-A722-23A769C31190}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="1db1eb16-7f87-45b5-a5c6-bd3f038db8d0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="3ebfc1ff-6854-40f8-8577-9c1c65c79578"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated scripts and outputs
</commit_message>
<xml_diff>
--- a/CDE_ID_detective_revamp/KnowledgeBase/Compiled_CORE_CDEs list_English_one sheet_as of 2025-01-28.xlsx
+++ b/CDE_ID_detective_revamp/KnowledgeBase/Compiled_CORE_CDEs list_English_one sheet_as of 2025-01-28.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmaefos\Code Stuffs\CDE_detective\CDE_ID_detective_revamp\KnowledgeBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557A7513-1F25-4B5D-A687-6554F651F309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5A277D-0037-4837-8636-78F4A11B6C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38505" yWindow="6465" windowWidth="20265" windowHeight="20985" xr2:uid="{35A4921A-9D1F-4A50-94BD-2A3998B45EE8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{35A4921A-9D1F-4A50-94BD-2A3998B45EE8}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7039" uniqueCount="1249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6999" uniqueCount="1249">
   <si>
     <t>Study Population Focus</t>
   </si>
@@ -4601,7 +4601,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Liezl Mae Fos" refreshedDate="45686.356838078704" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="435" xr:uid="{CA1B84A7-A9F9-4FF2-94BB-66C8FC57C7B7}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Liezl Mae Fos" refreshedDate="45688.437328935186" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="435" xr:uid="{CA1B84A7-A9F9-4FF2-94BB-66C8FC57C7B7}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:X1048576" sheet="ALL"/>
   </cacheSource>
@@ -16662,7 +16662,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{06BF0BB1-AF18-42F5-A5F1-83AA7DF4D85D}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:A80" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <location ref="A3:A40" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="24">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -16672,7 +16672,7 @@
         <item sd="0" x="1"/>
         <item sd="0" x="2"/>
         <item sd="0" x="0"/>
-        <item x="3"/>
+        <item sd="0" x="3"/>
         <item sd="0" m="1" x="29"/>
         <item sd="0" x="4"/>
         <item sd="0" m="1" x="30"/>
@@ -16690,7 +16690,7 @@
         <item sd="0" x="15"/>
         <item sd="0" m="1" x="31"/>
         <item sd="0" x="17"/>
-        <item sd="0" x="18"/>
+        <item x="18"/>
         <item sd="0" x="19"/>
         <item sd="0" x="20"/>
         <item sd="0" x="21"/>
@@ -17044,25 +17044,25 @@
         <item sd="0" x="56"/>
         <item sd="0" x="57"/>
         <item sd="0" x="58"/>
-        <item x="62"/>
-        <item x="63"/>
-        <item x="64"/>
-        <item x="65"/>
-        <item x="66"/>
-        <item x="67"/>
-        <item x="68"/>
-        <item x="69"/>
-        <item x="129"/>
-        <item x="130"/>
-        <item x="131"/>
-        <item x="132"/>
-        <item x="133"/>
-        <item x="134"/>
-        <item x="135"/>
-        <item x="136"/>
-        <item x="137"/>
-        <item x="183"/>
-        <item x="184"/>
+        <item sd="0" x="62"/>
+        <item sd="0" x="63"/>
+        <item sd="0" x="64"/>
+        <item sd="0" x="65"/>
+        <item sd="0" x="66"/>
+        <item sd="0" x="67"/>
+        <item sd="0" x="68"/>
+        <item sd="0" x="69"/>
+        <item sd="0" x="129"/>
+        <item sd="0" x="130"/>
+        <item sd="0" x="131"/>
+        <item sd="0" x="132"/>
+        <item sd="0" x="133"/>
+        <item sd="0" x="134"/>
+        <item sd="0" x="135"/>
+        <item sd="0" x="136"/>
+        <item sd="0" x="137"/>
+        <item sd="0" x="183"/>
+        <item sd="0" x="184"/>
         <item t="default" sd="0"/>
       </items>
     </pivotField>
@@ -17377,7 +17377,7 @@
     <field x="10"/>
     <field x="11"/>
   </rowFields>
-  <rowItems count="77">
+  <rowItems count="37">
     <i>
       <x v="1"/>
     </i>
@@ -17389,153 +17389,6 @@
     </i>
     <i>
       <x v="4"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i r="1">
-      <x v="22"/>
-    </i>
-    <i r="1">
-      <x v="23"/>
-    </i>
-    <i r="1">
-      <x v="33"/>
-    </i>
-    <i r="1">
-      <x v="42"/>
-    </i>
-    <i r="1">
-      <x v="43"/>
-    </i>
-    <i r="1">
-      <x v="44"/>
-    </i>
-    <i r="1">
-      <x v="45"/>
-    </i>
-    <i r="1">
-      <x v="46"/>
-    </i>
-    <i r="1">
-      <x v="47"/>
-    </i>
-    <i r="1">
-      <x v="48"/>
-    </i>
-    <i r="1">
-      <x v="49"/>
-    </i>
-    <i r="1">
-      <x v="50"/>
-    </i>
-    <i r="1">
-      <x v="54"/>
-    </i>
-    <i r="1">
-      <x v="55"/>
-    </i>
-    <i r="1">
-      <x v="56"/>
-    </i>
-    <i r="1">
-      <x v="57"/>
-    </i>
-    <i r="1">
-      <x v="58"/>
-    </i>
-    <i r="1">
-      <x v="59"/>
-    </i>
-    <i r="1">
-      <x v="76"/>
-    </i>
-    <i r="1">
-      <x v="77"/>
-    </i>
-    <i r="1">
-      <x v="78"/>
-    </i>
-    <i r="1">
-      <x v="138"/>
-    </i>
-    <i r="1">
-      <x v="139"/>
-    </i>
-    <i r="1">
-      <x v="140"/>
-    </i>
-    <i r="1">
-      <x v="142"/>
-    </i>
-    <i r="1">
-      <x v="149"/>
-    </i>
-    <i r="1">
-      <x v="150"/>
-    </i>
-    <i r="1">
-      <x v="151"/>
-    </i>
-    <i r="1">
-      <x v="152"/>
-    </i>
-    <i r="1">
-      <x v="154"/>
-    </i>
-    <i r="1">
-      <x v="155"/>
-    </i>
-    <i r="1">
-      <x v="156"/>
-    </i>
-    <i r="1">
-      <x v="157"/>
-    </i>
-    <i r="1">
-      <x v="158"/>
-    </i>
-    <i r="1">
-      <x v="159"/>
-    </i>
-    <i r="1">
-      <x v="160"/>
-    </i>
-    <i r="1">
-      <x v="161"/>
-    </i>
-    <i r="1">
-      <x v="162"/>
-    </i>
-    <i r="1">
-      <x v="163"/>
-    </i>
-    <i r="1">
-      <x v="164"/>
-    </i>
-    <i r="1">
-      <x v="165"/>
     </i>
     <i>
       <x v="6"/>
@@ -17581,6 +17434,33 @@
     </i>
     <i>
       <x v="22"/>
+    </i>
+    <i r="1">
+      <x v="120"/>
+    </i>
+    <i r="1">
+      <x v="121"/>
+    </i>
+    <i r="1">
+      <x v="174"/>
+    </i>
+    <i r="1">
+      <x v="175"/>
+    </i>
+    <i r="1">
+      <x v="176"/>
+    </i>
+    <i r="1">
+      <x v="177"/>
+    </i>
+    <i r="1">
+      <x v="178"/>
+    </i>
+    <i r="1">
+      <x v="179"/>
+    </i>
+    <i r="1">
+      <x v="180"/>
     </i>
     <i>
       <x v="23"/>
@@ -17942,22 +17822,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F8D453-0289-4E16-AB7B-CD7D302713CA}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Y435"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A371" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E381" sqref="E381"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14.86328125" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="14.46484375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="30.9296875" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.3984375" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43.6640625" style="8" customWidth="1"/>
     <col min="6" max="6" width="20.73046875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="55.3984375" style="8" customWidth="1"/>
     <col min="8" max="8" width="28.06640625" style="8" customWidth="1"/>
     <col min="9" max="9" width="28.86328125" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.86328125" style="8" bestFit="1" customWidth="1"/>
@@ -18777,7 +18658,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A18" s="8" t="s">
         <v>22</v>
       </c>
@@ -18841,7 +18722,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A19" s="8" t="s">
         <v>22</v>
       </c>
@@ -18894,7 +18775,7 @@
       <c r="W19" s="9"/>
       <c r="X19" s="9"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A20" s="8" t="s">
         <v>22</v>
       </c>
@@ -18957,7 +18838,7 @@
       <c r="W20" s="9"/>
       <c r="X20" s="9"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
         <v>22</v>
       </c>
@@ -19024,7 +18905,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A22" s="8" t="s">
         <v>22</v>
       </c>
@@ -19084,7 +18965,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A23" s="8" t="s">
         <v>22</v>
       </c>
@@ -19147,7 +19028,7 @@
       <c r="W23" s="9"/>
       <c r="X23" s="9"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A24" s="8" t="s">
         <v>22</v>
       </c>
@@ -19210,7 +19091,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A25" s="8" t="s">
         <v>22</v>
       </c>
@@ -19273,7 +19154,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A26" s="8" t="s">
         <v>22</v>
       </c>
@@ -19336,7 +19217,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A27" s="8" t="s">
         <v>22</v>
       </c>
@@ -19399,7 +19280,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A28" s="8" t="s">
         <v>22</v>
       </c>
@@ -19462,7 +19343,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A29" s="8" t="s">
         <v>22</v>
       </c>
@@ -19525,7 +19406,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A30" s="8" t="s">
         <v>22</v>
       </c>
@@ -19588,7 +19469,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A31" s="8" t="s">
         <v>22</v>
       </c>
@@ -19655,7 +19536,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A32" s="8" t="s">
         <v>22</v>
       </c>
@@ -19724,7 +19605,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A33" s="8" t="s">
         <v>22</v>
       </c>
@@ -19791,7 +19672,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A34" s="8" t="s">
         <v>22</v>
       </c>
@@ -19849,7 +19730,7 @@
       </c>
       <c r="U34" s="9"/>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A35" s="8" t="s">
         <v>22</v>
       </c>
@@ -19903,7 +19784,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A36" s="8" t="s">
         <v>22</v>
       </c>
@@ -19952,7 +19833,7 @@
       <c r="W36" s="9"/>
       <c r="X36" s="9"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A37" s="8" t="s">
         <v>22</v>
       </c>
@@ -20009,7 +19890,7 @@
       <c r="W37" s="9"/>
       <c r="X37" s="9"/>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A38" s="8" t="s">
         <v>22</v>
       </c>
@@ -20063,7 +19944,7 @@
       <c r="W38" s="9"/>
       <c r="X38" s="9"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A39" s="8" t="s">
         <v>22</v>
       </c>
@@ -20118,7 +19999,7 @@
       <c r="W39" s="9"/>
       <c r="X39" s="9"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A40" s="8" t="s">
         <v>202</v>
       </c>
@@ -20186,7 +20067,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A41" s="8" t="s">
         <v>202</v>
       </c>
@@ -20244,7 +20125,7 @@
       <c r="X41" s="9"/>
       <c r="Y41" s="9"/>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A42" s="8" t="s">
         <v>202</v>
       </c>
@@ -20302,7 +20183,7 @@
       <c r="X42" s="9"/>
       <c r="Y42" s="9"/>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A43" s="8" t="s">
         <v>202</v>
       </c>
@@ -20372,7 +20253,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A44" s="8" t="s">
         <v>202</v>
       </c>
@@ -20444,7 +20325,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A45" s="8" t="s">
         <v>202</v>
       </c>
@@ -20496,7 +20377,7 @@
       <c r="X45" s="9"/>
       <c r="Y45" s="9"/>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A46" s="8" t="s">
         <v>202</v>
       </c>
@@ -20562,7 +20443,7 @@
       <c r="X46" s="9"/>
       <c r="Y46" s="9"/>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A47" s="8" t="s">
         <v>202</v>
       </c>
@@ -20628,7 +20509,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A48" s="8" t="s">
         <v>202</v>
       </c>
@@ -20694,7 +20575,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A49" s="8" t="s">
         <v>202</v>
       </c>
@@ -20760,7 +20641,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A50" s="8" t="s">
         <v>202</v>
       </c>
@@ -20826,7 +20707,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A51" s="8" t="s">
         <v>202</v>
       </c>
@@ -20892,7 +20773,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A52" s="8" t="s">
         <v>202</v>
       </c>
@@ -20958,7 +20839,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A53" s="8" t="s">
         <v>202</v>
       </c>
@@ -21024,7 +20905,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A54" s="8" t="s">
         <v>202</v>
       </c>
@@ -21082,7 +20963,7 @@
       <c r="X54" s="9"/>
       <c r="Y54" s="9"/>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A55" s="8" t="s">
         <v>202</v>
       </c>
@@ -21140,7 +21021,7 @@
       <c r="X55" s="9"/>
       <c r="Y55" s="9"/>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A56" s="8" t="s">
         <v>202</v>
       </c>
@@ -21204,7 +21085,7 @@
       <c r="X56" s="9"/>
       <c r="Y56" s="9"/>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A57" s="8" t="s">
         <v>202</v>
       </c>
@@ -21258,7 +21139,7 @@
       <c r="X57" s="9"/>
       <c r="Y57" s="9"/>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A58" s="8" t="s">
         <v>202</v>
       </c>
@@ -21324,7 +21205,7 @@
       <c r="X58" s="9"/>
       <c r="Y58" s="9"/>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A59" s="8" t="s">
         <v>202</v>
       </c>
@@ -21390,7 +21271,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A60" s="8" t="s">
         <v>202</v>
       </c>
@@ -21456,7 +21337,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A61" s="8" t="s">
         <v>202</v>
       </c>
@@ -21522,7 +21403,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A62" s="8" t="s">
         <v>202</v>
       </c>
@@ -21588,7 +21469,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A63" s="8" t="s">
         <v>202</v>
       </c>
@@ -21654,7 +21535,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A64" s="8" t="s">
         <v>202</v>
       </c>
@@ -21720,7 +21601,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A65" s="8" t="s">
         <v>202</v>
       </c>
@@ -21786,7 +21667,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A66" s="8" t="s">
         <v>202</v>
       </c>
@@ -21856,7 +21737,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A67" s="8" t="s">
         <v>202</v>
       </c>
@@ -21928,7 +21809,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A68" s="8" t="s">
         <v>202</v>
       </c>
@@ -21998,7 +21879,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A69" s="8" t="s">
         <v>202</v>
       </c>
@@ -22068,7 +21949,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A70" s="8" t="s">
         <v>202</v>
       </c>
@@ -22140,7 +22021,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A71" s="8" t="s">
         <v>202</v>
       </c>
@@ -22206,7 +22087,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A72" s="8" t="s">
         <v>202</v>
       </c>
@@ -22260,7 +22141,7 @@
       <c r="X72" s="9"/>
       <c r="Y72" s="9"/>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A73" s="8" t="s">
         <v>202</v>
       </c>
@@ -22318,7 +22199,7 @@
       <c r="X73" s="9"/>
       <c r="Y73" s="9"/>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A74" s="8" t="s">
         <v>202</v>
       </c>
@@ -22374,7 +22255,7 @@
       <c r="X74" s="9"/>
       <c r="Y74" s="9"/>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A75" s="8" t="s">
         <v>202</v>
       </c>
@@ -22430,7 +22311,7 @@
       <c r="X75" s="15"/>
       <c r="Y75" s="15"/>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A76" s="8" t="s">
         <v>22</v>
       </c>
@@ -22489,7 +22370,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A77" s="8" t="s">
         <v>22</v>
       </c>
@@ -22548,7 +22429,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A78" s="8" t="s">
         <v>22</v>
       </c>
@@ -22607,7 +22488,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A79" s="8" t="s">
         <v>22</v>
       </c>
@@ -22666,7 +22547,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A80" s="8" t="s">
         <v>22</v>
       </c>
@@ -22725,7 +22606,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A81" s="8" t="s">
         <v>22</v>
       </c>
@@ -22784,7 +22665,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A82" s="8" t="s">
         <v>22</v>
       </c>
@@ -22843,7 +22724,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A83" s="8" t="s">
         <v>22</v>
       </c>
@@ -22902,7 +22783,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A84" s="8" t="s">
         <v>22</v>
       </c>
@@ -22961,7 +22842,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A85" s="8" t="s">
         <v>22</v>
       </c>
@@ -23016,7 +22897,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A86" s="8" t="s">
         <v>22</v>
       </c>
@@ -23071,7 +22952,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A87" s="8" t="s">
         <v>22</v>
       </c>
@@ -23125,7 +23006,7 @@
       <c r="X87" s="15"/>
       <c r="Y87" s="15"/>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A88" s="8" t="s">
         <v>1016</v>
       </c>
@@ -23181,7 +23062,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A89" s="8" t="s">
         <v>1016</v>
       </c>
@@ -23237,7 +23118,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A90" s="8" t="s">
         <v>1016</v>
       </c>
@@ -23287,7 +23168,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A91" s="8" t="s">
         <v>998</v>
       </c>
@@ -23343,7 +23224,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A92" s="8" t="s">
         <v>998</v>
       </c>
@@ -23399,7 +23280,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A93" s="8" t="s">
         <v>998</v>
       </c>
@@ -23449,7 +23330,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A94" s="8" t="s">
         <v>320</v>
       </c>
@@ -23505,7 +23386,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A95" s="8" t="s">
         <v>320</v>
       </c>
@@ -23561,7 +23442,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A96" s="8" t="s">
         <v>320</v>
       </c>
@@ -23611,7 +23492,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A97" s="8" t="s">
         <v>536</v>
       </c>
@@ -23667,7 +23548,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A98" s="8" t="s">
         <v>536</v>
       </c>
@@ -23723,7 +23604,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A99" s="8" t="s">
         <v>536</v>
       </c>
@@ -23773,7 +23654,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A100" s="8" t="s">
         <v>998</v>
       </c>
@@ -23829,7 +23710,7 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A101" s="8" t="s">
         <v>998</v>
       </c>
@@ -23885,7 +23766,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A102" s="8" t="s">
         <v>998</v>
       </c>
@@ -23938,7 +23819,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A103" s="8" t="s">
         <v>998</v>
       </c>
@@ -23991,7 +23872,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A104" s="8" t="s">
         <v>998</v>
       </c>
@@ -24044,7 +23925,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A105" s="8" t="s">
         <v>998</v>
       </c>
@@ -24097,7 +23978,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A106" s="8" t="s">
         <v>998</v>
       </c>
@@ -24150,7 +24031,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A107" s="8" t="s">
         <v>998</v>
       </c>
@@ -24200,7 +24081,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A108" s="8" t="s">
         <v>320</v>
       </c>
@@ -24256,7 +24137,7 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="109" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A109" s="8" t="s">
         <v>320</v>
       </c>
@@ -24312,7 +24193,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A110" s="8" t="s">
         <v>320</v>
       </c>
@@ -24365,7 +24246,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="111" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A111" s="8" t="s">
         <v>320</v>
       </c>
@@ -24418,7 +24299,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="112" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A112" s="8" t="s">
         <v>320</v>
       </c>
@@ -24471,7 +24352,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A113" s="8" t="s">
         <v>320</v>
       </c>
@@ -24524,7 +24405,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A114" s="8" t="s">
         <v>320</v>
       </c>
@@ -24577,7 +24458,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A115" s="8" t="s">
         <v>320</v>
       </c>
@@ -24627,7 +24508,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A116" s="8" t="s">
         <v>1164</v>
       </c>
@@ -24683,7 +24564,7 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A117" s="8" t="s">
         <v>1164</v>
       </c>
@@ -24739,7 +24620,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A118" s="8" t="s">
         <v>1164</v>
       </c>
@@ -24792,7 +24673,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A119" s="8" t="s">
         <v>1164</v>
       </c>
@@ -24845,7 +24726,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="120" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A120" s="8" t="s">
         <v>1164</v>
       </c>
@@ -24898,7 +24779,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="121" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A121" s="8" t="s">
         <v>1164</v>
       </c>
@@ -24951,7 +24832,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="122" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A122" s="8" t="s">
         <v>1164</v>
       </c>
@@ -25004,7 +24885,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="123" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A123" s="8" t="s">
         <v>1164</v>
       </c>
@@ -25054,7 +24935,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="124" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A124" s="8" t="s">
         <v>1165</v>
       </c>
@@ -25110,7 +24991,7 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="125" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A125" s="8" t="s">
         <v>1165</v>
       </c>
@@ -25166,7 +25047,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="126" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A126" s="8" t="s">
         <v>1165</v>
       </c>
@@ -25219,7 +25100,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="127" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A127" s="8" t="s">
         <v>1165</v>
       </c>
@@ -25272,7 +25153,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="128" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A128" s="8" t="s">
         <v>1165</v>
       </c>
@@ -25325,7 +25206,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="129" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A129" s="8" t="s">
         <v>1165</v>
       </c>
@@ -25378,7 +25259,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="130" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A130" s="8" t="s">
         <v>1165</v>
       </c>
@@ -25431,7 +25312,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="131" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A131" s="8" t="s">
         <v>1165</v>
       </c>
@@ -25481,7 +25362,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="132" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A132" s="8" t="s">
         <v>536</v>
       </c>
@@ -25531,7 +25412,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="133" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A133" s="8" t="s">
         <v>536</v>
       </c>
@@ -25581,7 +25462,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="134" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A134" s="8" t="s">
         <v>536</v>
       </c>
@@ -25631,7 +25512,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="135" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A135" s="8" t="s">
         <v>536</v>
       </c>
@@ -25681,7 +25562,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="136" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A136" s="8" t="s">
         <v>536</v>
       </c>
@@ -25731,7 +25612,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="137" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A137" s="8" t="s">
         <v>536</v>
       </c>
@@ -25781,7 +25662,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="138" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A138" s="8" t="s">
         <v>536</v>
       </c>
@@ -25831,7 +25712,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="139" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A139" s="8" t="s">
         <v>536</v>
       </c>
@@ -25881,7 +25762,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="140" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A140" s="8" t="s">
         <v>536</v>
       </c>
@@ -25931,7 +25812,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="141" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A141" s="8" t="s">
         <v>536</v>
       </c>
@@ -25981,7 +25862,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="142" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A142" s="8" t="s">
         <v>536</v>
       </c>
@@ -26031,7 +25912,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="143" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A143" s="8" t="s">
         <v>536</v>
       </c>
@@ -26081,7 +25962,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="144" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A144" s="8" t="s">
         <v>536</v>
       </c>
@@ -26131,7 +26012,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="145" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A145" s="8" t="s">
         <v>536</v>
       </c>
@@ -26181,7 +26062,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="146" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A146" s="8" t="s">
         <v>536</v>
       </c>
@@ -26231,7 +26112,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="147" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A147" s="8" t="s">
         <v>536</v>
       </c>
@@ -26281,7 +26162,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="148" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A148" s="8" t="s">
         <v>1016</v>
       </c>
@@ -26331,7 +26212,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="149" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A149" s="8" t="s">
         <v>1016</v>
       </c>
@@ -26381,7 +26262,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="150" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A150" s="8" t="s">
         <v>1016</v>
       </c>
@@ -26431,7 +26312,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="151" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A151" s="8" t="s">
         <v>1016</v>
       </c>
@@ -26481,7 +26362,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="152" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A152" s="8" t="s">
         <v>1016</v>
       </c>
@@ -26531,7 +26412,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="153" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A153" s="8" t="s">
         <v>1016</v>
       </c>
@@ -26581,7 +26462,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="154" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A154" s="8" t="s">
         <v>1016</v>
       </c>
@@ -26631,7 +26512,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="155" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A155" s="8" t="s">
         <v>1016</v>
       </c>
@@ -26681,7 +26562,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="156" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A156" s="8" t="s">
         <v>1016</v>
       </c>
@@ -26731,7 +26612,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="157" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A157" s="8" t="s">
         <v>1016</v>
       </c>
@@ -26781,7 +26662,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="158" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A158" s="8" t="s">
         <v>1016</v>
       </c>
@@ -26831,7 +26712,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="159" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A159" s="8" t="s">
         <v>1016</v>
       </c>
@@ -26881,7 +26762,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="160" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A160" s="8" t="s">
         <v>1016</v>
       </c>
@@ -26931,7 +26812,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="161" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A161" s="8" t="s">
         <v>1016</v>
       </c>
@@ -26981,7 +26862,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="162" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A162" s="8" t="s">
         <v>1016</v>
       </c>
@@ -27031,7 +26912,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="163" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A163" s="8" t="s">
         <v>1016</v>
       </c>
@@ -27081,7 +26962,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="164" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A164" s="8" t="s">
         <v>320</v>
       </c>
@@ -27095,7 +26976,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="165" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A165" s="8" t="s">
         <v>998</v>
       </c>
@@ -27109,7 +26990,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="166" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A166" s="8" t="s">
         <v>320</v>
       </c>
@@ -27123,7 +27004,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="167" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A167" s="8" t="s">
         <v>998</v>
       </c>
@@ -27137,7 +27018,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="168" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A168" s="8" t="s">
         <v>536</v>
       </c>
@@ -27190,7 +27071,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="169" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A169" s="8" t="s">
         <v>536</v>
       </c>
@@ -27243,7 +27124,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="170" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A170" s="8" t="s">
         <v>536</v>
       </c>
@@ -27296,7 +27177,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="171" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A171" s="8" t="s">
         <v>536</v>
       </c>
@@ -27349,7 +27230,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="172" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A172" s="8" t="s">
         <v>536</v>
       </c>
@@ -27402,7 +27283,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="173" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A173" s="8" t="s">
         <v>536</v>
       </c>
@@ -27455,7 +27336,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="174" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A174" s="8" t="s">
         <v>536</v>
       </c>
@@ -27508,7 +27389,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="175" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A175" s="8" t="s">
         <v>536</v>
       </c>
@@ -27561,7 +27442,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="176" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A176" s="8" t="s">
         <v>536</v>
       </c>
@@ -27614,7 +27495,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="177" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A177" s="8" t="s">
         <v>536</v>
       </c>
@@ -27667,7 +27548,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="178" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A178" s="8" t="s">
         <v>536</v>
       </c>
@@ -27720,7 +27601,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="179" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A179" s="8" t="s">
         <v>536</v>
       </c>
@@ -27773,7 +27654,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="180" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A180" s="8" t="s">
         <v>536</v>
       </c>
@@ -27826,7 +27707,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="181" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A181" s="8" t="s">
         <v>536</v>
       </c>
@@ -27876,7 +27757,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="182" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A182" s="8" t="s">
         <v>536</v>
       </c>
@@ -27926,7 +27807,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="183" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A183" s="8" t="s">
         <v>536</v>
       </c>
@@ -27976,7 +27857,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="184" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A184" s="8" t="s">
         <v>536</v>
       </c>
@@ -28026,7 +27907,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="185" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A185" s="8" t="s">
         <v>1016</v>
       </c>
@@ -28079,7 +27960,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="186" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A186" s="8" t="s">
         <v>1016</v>
       </c>
@@ -28132,7 +28013,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="187" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A187" s="8" t="s">
         <v>1016</v>
       </c>
@@ -28185,7 +28066,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="188" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A188" s="8" t="s">
         <v>1016</v>
       </c>
@@ -28238,7 +28119,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="189" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A189" s="8" t="s">
         <v>1016</v>
       </c>
@@ -28291,7 +28172,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="190" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A190" s="8" t="s">
         <v>1016</v>
       </c>
@@ -28344,7 +28225,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="191" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A191" s="8" t="s">
         <v>1016</v>
       </c>
@@ -28397,7 +28278,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="192" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A192" s="8" t="s">
         <v>1016</v>
       </c>
@@ -28450,7 +28331,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="193" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A193" s="8" t="s">
         <v>1016</v>
       </c>
@@ -28503,7 +28384,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="194" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A194" s="8" t="s">
         <v>1016</v>
       </c>
@@ -28556,7 +28437,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="195" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A195" s="8" t="s">
         <v>1016</v>
       </c>
@@ -28609,7 +28490,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="196" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A196" s="8" t="s">
         <v>1016</v>
       </c>
@@ -28662,7 +28543,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="197" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A197" s="8" t="s">
         <v>1016</v>
       </c>
@@ -28715,7 +28596,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="198" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A198" s="8" t="s">
         <v>1016</v>
       </c>
@@ -28765,7 +28646,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="199" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A199" s="8" t="s">
         <v>1016</v>
       </c>
@@ -28815,7 +28696,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="200" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A200" s="8" t="s">
         <v>1016</v>
       </c>
@@ -28865,7 +28746,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="201" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A201" s="8" t="s">
         <v>1016</v>
       </c>
@@ -28915,7 +28796,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="202" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A202" s="8" t="s">
         <v>536</v>
       </c>
@@ -28968,7 +28849,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="203" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A203" s="8" t="s">
         <v>536</v>
       </c>
@@ -29021,7 +28902,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="204" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A204" s="8" t="s">
         <v>536</v>
       </c>
@@ -29074,7 +28955,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="205" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A205" s="8" t="s">
         <v>536</v>
       </c>
@@ -29127,7 +29008,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="206" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A206" s="8" t="s">
         <v>536</v>
       </c>
@@ -29180,7 +29061,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="207" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A207" s="8" t="s">
         <v>536</v>
       </c>
@@ -29233,7 +29114,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="208" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A208" s="8" t="s">
         <v>536</v>
       </c>
@@ -29286,7 +29167,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="209" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A209" s="8" t="s">
         <v>536</v>
       </c>
@@ -29339,7 +29220,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="210" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A210" s="8" t="s">
         <v>536</v>
       </c>
@@ -29392,7 +29273,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="211" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A211" s="8" t="s">
         <v>536</v>
       </c>
@@ -29445,7 +29326,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="212" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A212" s="8" t="s">
         <v>536</v>
       </c>
@@ -29498,7 +29379,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="213" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A213" s="8" t="s">
         <v>536</v>
       </c>
@@ -29551,7 +29432,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="214" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A214" s="8" t="s">
         <v>536</v>
       </c>
@@ -29604,7 +29485,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="215" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A215" s="8" t="s">
         <v>536</v>
       </c>
@@ -29654,7 +29535,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="216" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A216" s="8" t="s">
         <v>536</v>
       </c>
@@ -29704,7 +29585,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="217" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A217" s="8" t="s">
         <v>536</v>
       </c>
@@ -29754,7 +29635,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="218" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A218" s="8" t="s">
         <v>536</v>
       </c>
@@ -29804,7 +29685,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="219" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A219" s="8" t="s">
         <v>1016</v>
       </c>
@@ -29857,7 +29738,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="220" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A220" s="8" t="s">
         <v>1016</v>
       </c>
@@ -29910,7 +29791,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="221" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A221" s="8" t="s">
         <v>1016</v>
       </c>
@@ -29963,7 +29844,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="222" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A222" s="8" t="s">
         <v>1016</v>
       </c>
@@ -30016,7 +29897,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="223" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A223" s="8" t="s">
         <v>1016</v>
       </c>
@@ -30069,7 +29950,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="224" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A224" s="8" t="s">
         <v>1016</v>
       </c>
@@ -30122,7 +30003,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="225" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A225" s="8" t="s">
         <v>1016</v>
       </c>
@@ -30175,7 +30056,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="226" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A226" s="8" t="s">
         <v>1016</v>
       </c>
@@ -30228,7 +30109,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="227" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A227" s="8" t="s">
         <v>1016</v>
       </c>
@@ -30281,7 +30162,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="228" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A228" s="8" t="s">
         <v>1016</v>
       </c>
@@ -30334,7 +30215,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="229" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A229" s="8" t="s">
         <v>1016</v>
       </c>
@@ -30387,7 +30268,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="230" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A230" s="8" t="s">
         <v>1016</v>
       </c>
@@ -30440,7 +30321,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="231" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A231" s="8" t="s">
         <v>1016</v>
       </c>
@@ -30493,7 +30374,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="232" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A232" s="8" t="s">
         <v>1016</v>
       </c>
@@ -30543,7 +30424,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="233" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A233" s="8" t="s">
         <v>1016</v>
       </c>
@@ -30593,7 +30474,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="234" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A234" s="8" t="s">
         <v>1016</v>
       </c>
@@ -30643,7 +30524,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="235" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A235" s="8" t="s">
         <v>1016</v>
       </c>
@@ -30693,7 +30574,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="236" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A236" s="8" t="s">
         <v>536</v>
       </c>
@@ -30707,7 +30588,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="237" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A237" s="8" t="s">
         <v>1016</v>
       </c>
@@ -30721,7 +30602,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="238" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A238" s="8" t="s">
         <v>320</v>
       </c>
@@ -30771,7 +30652,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="239" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A239" s="8" t="s">
         <v>320</v>
       </c>
@@ -30824,7 +30705,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="240" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A240" s="8" t="s">
         <v>320</v>
       </c>
@@ -30877,7 +30758,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="241" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A241" s="8" t="s">
         <v>320</v>
       </c>
@@ -30924,7 +30805,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="242" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A242" s="8" t="s">
         <v>320</v>
       </c>
@@ -30977,7 +30858,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="243" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A243" s="8" t="s">
         <v>536</v>
       </c>
@@ -31030,7 +30911,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="244" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A244" s="8" t="s">
         <v>998</v>
       </c>
@@ -31083,7 +30964,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="245" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A245" s="8" t="s">
         <v>1016</v>
       </c>
@@ -31136,7 +31017,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="246" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A246" s="8" t="s">
         <v>536</v>
       </c>
@@ -31189,7 +31070,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="247" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A247" s="8" t="s">
         <v>1016</v>
       </c>
@@ -31242,7 +31123,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="248" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A248" s="8" t="s">
         <v>320</v>
       </c>
@@ -31295,7 +31176,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="249" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A249" s="8" t="s">
         <v>320</v>
       </c>
@@ -31348,7 +31229,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="250" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A250" s="8" t="s">
         <v>320</v>
       </c>
@@ -31398,7 +31279,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="251" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A251" s="8" t="s">
         <v>536</v>
       </c>
@@ -31451,7 +31332,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="252" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A252" s="8" t="s">
         <v>536</v>
       </c>
@@ -31504,7 +31385,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="253" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A253" s="8" t="s">
         <v>536</v>
       </c>
@@ -31554,7 +31435,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="254" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A254" s="8" t="s">
         <v>998</v>
       </c>
@@ -31607,7 +31488,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="255" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A255" s="8" t="s">
         <v>998</v>
       </c>
@@ -31660,7 +31541,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="256" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A256" s="8" t="s">
         <v>998</v>
       </c>
@@ -31710,7 +31591,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="257" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A257" s="8" t="s">
         <v>1016</v>
       </c>
@@ -31763,7 +31644,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="258" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A258" s="8" t="s">
         <v>1016</v>
       </c>
@@ -31816,7 +31697,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="259" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A259" s="8" t="s">
         <v>1016</v>
       </c>
@@ -31866,7 +31747,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="260" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A260" s="8" t="s">
         <v>998</v>
       </c>
@@ -31922,7 +31803,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="261" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A261" s="8" t="s">
         <v>998</v>
       </c>
@@ -31978,7 +31859,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="262" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="262" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A262" s="8" t="s">
         <v>998</v>
       </c>
@@ -32034,7 +31915,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="263" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="263" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A263" s="8" t="s">
         <v>998</v>
       </c>
@@ -32090,7 +31971,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="264" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="264" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A264" s="8" t="s">
         <v>998</v>
       </c>
@@ -32146,7 +32027,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="265" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="265" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A265" s="8" t="s">
         <v>998</v>
       </c>
@@ -32202,7 +32083,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="266" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="266" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A266" s="8" t="s">
         <v>998</v>
       </c>
@@ -32258,7 +32139,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="267" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="267" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A267" s="8" t="s">
         <v>998</v>
       </c>
@@ -32314,7 +32195,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="268" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="268" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A268" s="8" t="s">
         <v>998</v>
       </c>
@@ -32361,7 +32242,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="269" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="269" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A269" s="8" t="s">
         <v>320</v>
       </c>
@@ -32417,7 +32298,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="270" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="270" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A270" s="8" t="s">
         <v>320</v>
       </c>
@@ -32473,7 +32354,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="271" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="271" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A271" s="8" t="s">
         <v>320</v>
       </c>
@@ -32529,7 +32410,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="272" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="272" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A272" s="8" t="s">
         <v>320</v>
       </c>
@@ -32585,7 +32466,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="273" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="273" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A273" s="8" t="s">
         <v>320</v>
       </c>
@@ -32641,7 +32522,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="274" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="274" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A274" s="8" t="s">
         <v>320</v>
       </c>
@@ -32697,7 +32578,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="275" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="275" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A275" s="8" t="s">
         <v>320</v>
       </c>
@@ -32753,7 +32634,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="276" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="276" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A276" s="8" t="s">
         <v>320</v>
       </c>
@@ -32809,7 +32690,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="277" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="277" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A277" s="8" t="s">
         <v>320</v>
       </c>
@@ -32856,7 +32737,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="278" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="278" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A278" s="8" t="s">
         <v>1164</v>
       </c>
@@ -32912,7 +32793,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="279" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="279" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A279" s="8" t="s">
         <v>1164</v>
       </c>
@@ -32968,7 +32849,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="280" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="280" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A280" s="8" t="s">
         <v>1164</v>
       </c>
@@ -33024,7 +32905,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="281" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="281" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A281" s="8" t="s">
         <v>1164</v>
       </c>
@@ -33080,7 +32961,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="282" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="282" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A282" s="8" t="s">
         <v>1164</v>
       </c>
@@ -33136,7 +33017,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="283" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="283" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A283" s="8" t="s">
         <v>1164</v>
       </c>
@@ -33192,7 +33073,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="284" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="284" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A284" s="8" t="s">
         <v>1164</v>
       </c>
@@ -33248,7 +33129,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="285" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="285" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A285" s="8" t="s">
         <v>1164</v>
       </c>
@@ -33304,7 +33185,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="286" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="286" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A286" s="8" t="s">
         <v>1164</v>
       </c>
@@ -33351,7 +33232,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="287" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="287" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A287" s="8" t="s">
         <v>1165</v>
       </c>
@@ -33407,7 +33288,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="288" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="288" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A288" s="8" t="s">
         <v>1165</v>
       </c>
@@ -33463,7 +33344,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="289" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="289" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A289" s="8" t="s">
         <v>1165</v>
       </c>
@@ -33519,7 +33400,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="290" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="290" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A290" s="8" t="s">
         <v>1165</v>
       </c>
@@ -33575,7 +33456,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="291" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="291" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A291" s="8" t="s">
         <v>1165</v>
       </c>
@@ -33631,7 +33512,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="292" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="292" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A292" s="8" t="s">
         <v>1165</v>
       </c>
@@ -33687,7 +33568,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="293" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="293" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A293" s="8" t="s">
         <v>1165</v>
       </c>
@@ -33743,7 +33624,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="294" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="294" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A294" s="8" t="s">
         <v>1165</v>
       </c>
@@ -33799,7 +33680,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="295" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="295" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A295" s="8" t="s">
         <v>1165</v>
       </c>
@@ -33846,7 +33727,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="296" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="296" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A296" s="8" t="s">
         <v>998</v>
       </c>
@@ -33902,7 +33783,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="297" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="297" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A297" s="8" t="s">
         <v>998</v>
       </c>
@@ -33958,7 +33839,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="298" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="298" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A298" s="8" t="s">
         <v>998</v>
       </c>
@@ -34014,7 +33895,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="299" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="299" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A299" s="8" t="s">
         <v>998</v>
       </c>
@@ -34070,7 +33951,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="300" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="300" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A300" s="8" t="s">
         <v>998</v>
       </c>
@@ -34126,7 +34007,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="301" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="301" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A301" s="8" t="s">
         <v>998</v>
       </c>
@@ -34182,7 +34063,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="302" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="302" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A302" s="8" t="s">
         <v>998</v>
       </c>
@@ -34238,7 +34119,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="303" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="303" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A303" s="8" t="s">
         <v>998</v>
       </c>
@@ -34294,7 +34175,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="304" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="304" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A304" s="8" t="s">
         <v>998</v>
       </c>
@@ -34347,7 +34228,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="305" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="305" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A305" s="8" t="s">
         <v>998</v>
       </c>
@@ -34394,7 +34275,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="306" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="306" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A306" s="8" t="s">
         <v>998</v>
       </c>
@@ -34450,7 +34331,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="307" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="307" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A307" s="8" t="s">
         <v>320</v>
       </c>
@@ -34506,7 +34387,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="308" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="308" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A308" s="8" t="s">
         <v>320</v>
       </c>
@@ -34562,7 +34443,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="309" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="309" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A309" s="8" t="s">
         <v>320</v>
       </c>
@@ -34618,7 +34499,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="310" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="310" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A310" s="8" t="s">
         <v>320</v>
       </c>
@@ -34674,7 +34555,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="311" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="311" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A311" s="8" t="s">
         <v>320</v>
       </c>
@@ -34730,7 +34611,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="312" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="312" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A312" s="8" t="s">
         <v>320</v>
       </c>
@@ -34786,7 +34667,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="313" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="313" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A313" s="8" t="s">
         <v>320</v>
       </c>
@@ -34842,7 +34723,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="314" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="314" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A314" s="8" t="s">
         <v>320</v>
       </c>
@@ -34898,7 +34779,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="315" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="315" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A315" s="8" t="s">
         <v>320</v>
       </c>
@@ -34951,7 +34832,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="316" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="316" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A316" s="8" t="s">
         <v>320</v>
       </c>
@@ -34998,7 +34879,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="317" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="317" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A317" s="8" t="s">
         <v>320</v>
       </c>
@@ -35054,7 +34935,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="318" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="318" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A318" s="8" t="s">
         <v>1164</v>
       </c>
@@ -35110,7 +34991,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="319" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="319" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A319" s="8" t="s">
         <v>1164</v>
       </c>
@@ -35166,7 +35047,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="320" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="320" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A320" s="8" t="s">
         <v>1164</v>
       </c>
@@ -35222,7 +35103,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="321" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="321" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A321" s="8" t="s">
         <v>1164</v>
       </c>
@@ -35278,7 +35159,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="322" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="322" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A322" s="8" t="s">
         <v>1164</v>
       </c>
@@ -35334,7 +35215,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="323" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="323" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A323" s="8" t="s">
         <v>1164</v>
       </c>
@@ -35390,7 +35271,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="324" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="324" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A324" s="8" t="s">
         <v>1164</v>
       </c>
@@ -35446,7 +35327,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="325" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="325" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A325" s="8" t="s">
         <v>1164</v>
       </c>
@@ -35502,7 +35383,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="326" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="326" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A326" s="8" t="s">
         <v>1164</v>
       </c>
@@ -35555,7 +35436,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="327" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="327" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A327" s="8" t="s">
         <v>1164</v>
       </c>
@@ -35602,7 +35483,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="328" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="328" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A328" s="8" t="s">
         <v>1164</v>
       </c>
@@ -35658,7 +35539,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="329" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="329" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A329" s="8" t="s">
         <v>1165</v>
       </c>
@@ -35714,7 +35595,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="330" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="330" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A330" s="8" t="s">
         <v>1165</v>
       </c>
@@ -35770,7 +35651,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="331" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="331" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A331" s="8" t="s">
         <v>1165</v>
       </c>
@@ -35826,7 +35707,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="332" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="332" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A332" s="8" t="s">
         <v>1165</v>
       </c>
@@ -35882,7 +35763,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="333" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="333" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A333" s="8" t="s">
         <v>1165</v>
       </c>
@@ -35938,7 +35819,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="334" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="334" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A334" s="8" t="s">
         <v>1165</v>
       </c>
@@ -35994,7 +35875,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="335" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="335" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A335" s="8" t="s">
         <v>1165</v>
       </c>
@@ -36050,7 +35931,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="336" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="336" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A336" s="8" t="s">
         <v>1165</v>
       </c>
@@ -36106,7 +35987,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="337" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="337" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A337" s="8" t="s">
         <v>1165</v>
       </c>
@@ -36159,7 +36040,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="338" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="338" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A338" s="8" t="s">
         <v>1165</v>
       </c>
@@ -36206,7 +36087,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="339" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="339" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A339" s="8" t="s">
         <v>1165</v>
       </c>
@@ -36262,7 +36143,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="340" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="340" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A340" s="8" t="s">
         <v>998</v>
       </c>
@@ -36312,7 +36193,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="341" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="341" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A341" s="8" t="s">
         <v>998</v>
       </c>
@@ -36362,7 +36243,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="342" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="342" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A342" s="8" t="s">
         <v>998</v>
       </c>
@@ -36412,7 +36293,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="343" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="343" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A343" s="8" t="s">
         <v>998</v>
       </c>
@@ -36462,7 +36343,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="344" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="344" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A344" s="8" t="s">
         <v>998</v>
       </c>
@@ -36512,7 +36393,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="345" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="345" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A345" s="8" t="s">
         <v>998</v>
       </c>
@@ -36562,7 +36443,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="346" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="346" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A346" s="8" t="s">
         <v>998</v>
       </c>
@@ -36609,7 +36490,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="347" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="347" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A347" s="8" t="s">
         <v>998</v>
       </c>
@@ -36653,7 +36534,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="348" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="348" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A348" s="8" t="s">
         <v>320</v>
       </c>
@@ -36703,7 +36584,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="349" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="349" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A349" s="8" t="s">
         <v>320</v>
       </c>
@@ -36753,7 +36634,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="350" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="350" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A350" s="8" t="s">
         <v>320</v>
       </c>
@@ -36803,7 +36684,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="351" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="351" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A351" s="8" t="s">
         <v>320</v>
       </c>
@@ -36853,7 +36734,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="352" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="352" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A352" s="8" t="s">
         <v>320</v>
       </c>
@@ -36903,7 +36784,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="353" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="353" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A353" s="8" t="s">
         <v>320</v>
       </c>
@@ -36953,7 +36834,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="354" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="354" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A354" s="8" t="s">
         <v>320</v>
       </c>
@@ -37000,7 +36881,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="355" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="355" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A355" s="8" t="s">
         <v>320</v>
       </c>
@@ -37044,7 +36925,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="356" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="356" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A356" s="8" t="s">
         <v>320</v>
       </c>
@@ -37097,7 +36978,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="357" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="357" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A357" s="8" t="s">
         <v>320</v>
       </c>
@@ -37150,7 +37031,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="358" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="358" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A358" s="8" t="s">
         <v>320</v>
       </c>
@@ -37203,7 +37084,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="359" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="359" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A359" s="8" t="s">
         <v>320</v>
       </c>
@@ -37256,7 +37137,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="360" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="360" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A360" s="8" t="s">
         <v>320</v>
       </c>
@@ -37309,7 +37190,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="361" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="361" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A361" s="8" t="s">
         <v>320</v>
       </c>
@@ -37362,7 +37243,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="362" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="362" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A362" s="8" t="s">
         <v>320</v>
       </c>
@@ -37409,7 +37290,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="363" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="363" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A363" s="8" t="s">
         <v>320</v>
       </c>
@@ -37453,7 +37334,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="364" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="364" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A364" s="8" t="s">
         <v>998</v>
       </c>
@@ -37506,7 +37387,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="365" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="365" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A365" s="8" t="s">
         <v>998</v>
       </c>
@@ -37559,7 +37440,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="366" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="366" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A366" s="8" t="s">
         <v>998</v>
       </c>
@@ -37612,7 +37493,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="367" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="367" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A367" s="8" t="s">
         <v>998</v>
       </c>
@@ -37665,7 +37546,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="368" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="368" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A368" s="8" t="s">
         <v>998</v>
       </c>
@@ -37718,7 +37599,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="369" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="369" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A369" s="8" t="s">
         <v>998</v>
       </c>
@@ -37771,7 +37652,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="370" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="370" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A370" s="8" t="s">
         <v>998</v>
       </c>
@@ -37818,7 +37699,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="371" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="371" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A371" s="8" t="s">
         <v>998</v>
       </c>
@@ -37862,7 +37743,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="372" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="372" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A372" s="8" t="s">
         <v>320</v>
       </c>
@@ -37906,7 +37787,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="373" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="373" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A373" s="8" t="s">
         <v>536</v>
       </c>
@@ -37950,7 +37831,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="374" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="374" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A374" s="8" t="s">
         <v>998</v>
       </c>
@@ -37994,7 +37875,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="375" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="375" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A375" s="8" t="s">
         <v>1016</v>
       </c>
@@ -38038,7 +37919,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="376" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="376" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A376" s="8" t="s">
         <v>536</v>
       </c>
@@ -38091,7 +37972,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="377" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="377" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A377" s="8" t="s">
         <v>536</v>
       </c>
@@ -38141,7 +38022,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="378" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="378" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A378" s="8" t="s">
         <v>536</v>
       </c>
@@ -38191,7 +38072,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="379" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="379" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A379" s="8" t="s">
         <v>536</v>
       </c>
@@ -38244,7 +38125,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="380" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="380" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A380" s="8" t="s">
         <v>536</v>
       </c>
@@ -38294,7 +38175,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="381" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="381" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A381" s="8" t="s">
         <v>536</v>
       </c>
@@ -38347,7 +38228,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="382" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="382" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A382" s="8" t="s">
         <v>536</v>
       </c>
@@ -38397,7 +38278,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="383" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="383" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A383" s="8" t="s">
         <v>536</v>
       </c>
@@ -38447,7 +38328,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="384" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="384" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A384" s="8" t="s">
         <v>536</v>
       </c>
@@ -38500,7 +38381,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="385" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="385" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A385" s="8" t="s">
         <v>536</v>
       </c>
@@ -38550,7 +38431,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="386" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="386" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A386" s="8" t="s">
         <v>536</v>
       </c>
@@ -38603,7 +38484,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="387" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="387" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A387" s="8" t="s">
         <v>536</v>
       </c>
@@ -38653,7 +38534,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="388" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="388" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A388" s="8" t="s">
         <v>536</v>
       </c>
@@ -38706,7 +38587,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="389" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="389" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A389" s="8" t="s">
         <v>536</v>
       </c>
@@ -38756,7 +38637,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="390" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="390" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A390" s="8" t="s">
         <v>536</v>
       </c>
@@ -38809,7 +38690,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="391" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="391" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A391" s="8" t="s">
         <v>536</v>
       </c>
@@ -38859,7 +38740,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="392" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="392" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A392" s="8" t="s">
         <v>536</v>
       </c>
@@ -38912,7 +38793,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="393" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="393" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A393" s="8" t="s">
         <v>536</v>
       </c>
@@ -38962,7 +38843,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="394" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="394" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A394" s="8" t="s">
         <v>536</v>
       </c>
@@ -39012,7 +38893,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="395" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="395" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A395" s="8" t="s">
         <v>536</v>
       </c>
@@ -39062,7 +38943,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="396" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="396" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A396" s="8" t="s">
         <v>536</v>
       </c>
@@ -39112,7 +38993,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="397" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="397" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A397" s="8" t="s">
         <v>536</v>
       </c>
@@ -39162,7 +39043,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="398" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="398" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A398" s="8" t="s">
         <v>1016</v>
       </c>
@@ -39215,7 +39096,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="399" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="399" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A399" s="8" t="s">
         <v>1016</v>
       </c>
@@ -39265,7 +39146,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="400" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="400" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A400" s="8" t="s">
         <v>1016</v>
       </c>
@@ -39315,7 +39196,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="401" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="401" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A401" s="8" t="s">
         <v>1016</v>
       </c>
@@ -39368,7 +39249,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="402" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="402" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A402" s="8" t="s">
         <v>1016</v>
       </c>
@@ -39418,7 +39299,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="403" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="403" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A403" s="8" t="s">
         <v>1016</v>
       </c>
@@ -39471,7 +39352,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="404" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="404" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A404" s="8" t="s">
         <v>1016</v>
       </c>
@@ -39521,7 +39402,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="405" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="405" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A405" s="8" t="s">
         <v>1016</v>
       </c>
@@ -39571,7 +39452,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="406" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="406" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A406" s="8" t="s">
         <v>1016</v>
       </c>
@@ -39624,7 +39505,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="407" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="407" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A407" s="8" t="s">
         <v>1016</v>
       </c>
@@ -39674,7 +39555,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="408" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="408" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A408" s="8" t="s">
         <v>1016</v>
       </c>
@@ -39727,7 +39608,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="409" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="409" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A409" s="8" t="s">
         <v>1016</v>
       </c>
@@ -39777,7 +39658,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="410" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="410" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A410" s="8" t="s">
         <v>1016</v>
       </c>
@@ -39830,7 +39711,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="411" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="411" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A411" s="8" t="s">
         <v>1016</v>
       </c>
@@ -39880,7 +39761,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="412" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="412" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A412" s="8" t="s">
         <v>1016</v>
       </c>
@@ -39933,7 +39814,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="413" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="413" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A413" s="8" t="s">
         <v>1016</v>
       </c>
@@ -39983,7 +39864,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="414" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="414" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A414" s="8" t="s">
         <v>1016</v>
       </c>
@@ -40036,7 +39917,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="415" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="415" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A415" s="8" t="s">
         <v>1016</v>
       </c>
@@ -40086,7 +39967,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="416" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="416" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A416" s="8" t="s">
         <v>1016</v>
       </c>
@@ -40136,7 +40017,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="417" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="417" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A417" s="8" t="s">
         <v>1016</v>
       </c>
@@ -40186,7 +40067,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="418" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="418" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A418" s="8" t="s">
         <v>1016</v>
       </c>
@@ -40236,7 +40117,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="419" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="419" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A419" s="8" t="s">
         <v>1016</v>
       </c>
@@ -40286,7 +40167,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="420" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="420" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A420" s="8" t="s">
         <v>320</v>
       </c>
@@ -40336,7 +40217,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="421" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="421" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A421" s="8" t="s">
         <v>320</v>
       </c>
@@ -40386,7 +40267,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="422" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="422" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A422" s="8" t="s">
         <v>320</v>
       </c>
@@ -40436,7 +40317,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="423" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="423" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A423" s="8" t="s">
         <v>320</v>
       </c>
@@ -40486,7 +40367,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="424" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="424" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A424" s="8" t="s">
         <v>320</v>
       </c>
@@ -40536,7 +40417,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="425" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="425" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A425" s="8" t="s">
         <v>320</v>
       </c>
@@ -40589,7 +40470,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="426" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="426" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A426" s="8" t="s">
         <v>998</v>
       </c>
@@ -40639,7 +40520,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="427" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="427" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A427" s="8" t="s">
         <v>998</v>
       </c>
@@ -40689,7 +40570,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="428" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="428" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A428" s="8" t="s">
         <v>998</v>
       </c>
@@ -40739,7 +40620,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="429" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="429" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A429" s="8" t="s">
         <v>998</v>
       </c>
@@ -40789,7 +40670,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="430" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="430" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A430" s="8" t="s">
         <v>998</v>
       </c>
@@ -40839,7 +40720,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="431" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="431" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A431" s="8" t="s">
         <v>998</v>
       </c>
@@ -40892,7 +40773,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="432" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="432" spans="1:24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A432" s="8" t="s">
         <v>998</v>
       </c>
@@ -40942,7 +40823,7 @@
         <v>1147</v>
       </c>
     </row>
-    <row r="433" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="433" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A433" s="8" t="s">
         <v>998</v>
       </c>
@@ -40992,7 +40873,7 @@
         <v>1147</v>
       </c>
     </row>
-    <row r="434" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="434" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A434" s="8" t="s">
         <v>320</v>
       </c>
@@ -41042,7 +40923,7 @@
         <v>1147</v>
       </c>
     </row>
-    <row r="435" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="435" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A435" s="8" t="s">
         <v>320</v>
       </c>
@@ -41094,6 +40975,13 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:Y435" xr:uid="{52F8D453-0289-4E16-AB7B-CD7D302713CA}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="BPI Pain Interference"/>
+        <filter val="BPI Pain Severity"/>
+        <filter val="Brief Pain Inventory (BPI)"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y431">
       <sortCondition ref="C2:C431"/>
     </sortState>
@@ -41115,10 +41003,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B03DD75-91C1-4925-A600-9AD1195ECA81}">
-  <dimension ref="A3:A80"/>
+  <dimension ref="A3:A40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -41152,367 +41040,167 @@
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A8" s="23" t="s">
-        <v>41</v>
+      <c r="A8" s="2" t="s">
+        <v>1001</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A9" s="23" t="s">
-        <v>250</v>
+      <c r="A9" s="2" t="s">
+        <v>1186</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A10" s="23" t="s">
-        <v>210</v>
+      <c r="A10" s="2" t="s">
+        <v>699</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A11" s="23" t="s">
-        <v>255</v>
+      <c r="A11" s="2" t="s">
+        <v>1248</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A12" s="23" t="s">
-        <v>93</v>
+      <c r="A12" s="2" t="s">
+        <v>1230</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A13" s="23" t="s">
-        <v>281</v>
+      <c r="A13" s="2" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A14" s="23" t="s">
-        <v>103</v>
+      <c r="A14" s="2" t="s">
+        <v>918</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A15" s="23" t="s">
-        <v>284</v>
+      <c r="A15" s="2" t="s">
+        <v>817</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A16" s="23" t="s">
-        <v>109</v>
+      <c r="A16" s="2" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" s="23" t="s">
-        <v>287</v>
+      <c r="A17" s="2" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" s="23" t="s">
-        <v>25</v>
+      <c r="A18" s="2" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" s="23" t="s">
-        <v>187</v>
+      <c r="A19" s="2" t="s">
+        <v>687</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A20" s="23" t="s">
-        <v>197</v>
+      <c r="A20" s="2" t="s">
+        <v>1017</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A21" s="23" t="s">
-        <v>167</v>
+      <c r="A21" s="2" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A22" s="23" t="s">
-        <v>125</v>
+      <c r="A22" s="2" t="s">
+        <v>1112</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" s="23" t="s">
-        <v>310</v>
+        <v>429</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" s="23" t="s">
-        <v>134</v>
+        <v>421</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="23" t="s">
-        <v>315</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" s="23" t="s">
-        <v>86</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" s="23" t="s">
-        <v>277</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" s="23" t="s">
-        <v>61</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" s="23" t="s">
-        <v>74</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" s="23" t="s">
-        <v>156</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" s="23" t="s">
-        <v>145</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A32" s="23" t="s">
-        <v>112</v>
+      <c r="A32" s="2" t="s">
+        <v>1166</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A33" s="23" t="s">
-        <v>290</v>
+      <c r="A33" s="2" t="s">
+        <v>1002</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A34" s="23" t="s">
-        <v>121</v>
+      <c r="A34" s="2" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A35" s="23" t="s">
-        <v>299</v>
+      <c r="A35" s="2" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A36" s="23" t="s">
-        <v>174</v>
+      <c r="A36" s="2" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A37" s="23" t="s">
-        <v>261</v>
+      <c r="A37" s="2" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A38" s="23" t="s">
-        <v>272</v>
+      <c r="A38" s="2" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A39" s="23" t="s">
-        <v>49</v>
+      <c r="A39" s="2" t="s">
+        <v>1232</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A40" s="23" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A41" s="23" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A42" s="23" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A43" s="23" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A44" s="23" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A45" s="23" t="s">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A46" s="23" t="s">
-        <v>1035</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A47" s="23" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A48" s="23" t="s">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A49" s="23" t="s">
-        <v>1056</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A50" s="23" t="s">
-        <v>1063</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A51" s="23" t="s">
-        <v>1070</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A52" s="23" t="s">
-        <v>1077</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A53" s="23" t="s">
-        <v>1084</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A54" s="23" t="s">
-        <v>1091</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A55" s="23" t="s">
-        <v>1096</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A56" s="23" t="s">
-        <v>1106</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A57" s="2" t="s">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A58" s="2" t="s">
-        <v>1186</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A59" s="2" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A60" s="2" t="s">
-        <v>1248</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A61" s="2" t="s">
-        <v>1230</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A62" s="2" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A63" s="2" t="s">
-        <v>918</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A64" s="2" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A65" s="2" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A66" s="2" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A67" s="2" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A68" s="2" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A69" s="2" t="s">
-        <v>1017</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A70" s="2" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A71" s="2" t="s">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A72" s="2" t="s">
-        <v>1166</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A73" s="2" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A74" s="2" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A75" s="2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A76" s="2" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A77" s="2" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A78" s="2" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A79" s="2" t="s">
-        <v>1232</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A80" s="2" t="s">
+      <c r="A40" s="2" t="s">
         <v>1022</v>
       </c>
     </row>
@@ -41522,20 +41210,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3ebfc1ff-6854-40f8-8577-9c1c65c79578" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3ebfc1ff-6854-40f8-8577-9c1c65c79578" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -41728,6 +41416,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DFF46F5-41AA-471B-8C04-D49580FCB34E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3DFAF0B-A9BC-422F-A722-23A769C31190}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -41740,14 +41436,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="3ebfc1ff-6854-40f8-8577-9c1c65c79578"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DFF46F5-41AA-471B-8C04-D49580FCB34E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>